<commit_message>
Updated sprint 106 actual and result
</commit_message>
<xml_diff>
--- a/Buyer hub/Inventory/Manual testcases/Inventory-SKU Listing.xlsx
+++ b/Buyer hub/Inventory/Manual testcases/Inventory-SKU Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Inventory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0165F999-9C98-4872-A831-B6FA15766039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F17E04C-2DFB-45A4-95AF-E65D7F34E027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>SL. No</t>
   </si>
@@ -246,9 +246,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">1.It shows Est.value at count, No.of items and Below par             2.Search SKU, All outlets, Status, Search,                                  </t>
-  </si>
-  <si>
     <t>SKU -&gt; All Outlets</t>
   </si>
   <si>
@@ -373,6 +370,15 @@
       </rPr>
       <t xml:space="preserve"> (as of stock count date).</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1.It shows Est.value at count, No.of items and Below par             2.Search SKU, All outlets, Status, Search and Export                              </t>
+  </si>
+  <si>
+    <t>It displayed the Total quantity and value</t>
+  </si>
+  <si>
+    <t>Once click the Export it downloaded Excel sheet in details</t>
   </si>
 </sst>
 </file>
@@ -810,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +962,7 @@
         <v>35</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>25</v>
@@ -999,10 +1005,10 @@
         <v>24</v>
       </c>
       <c r="D8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>41</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>29</v>
@@ -1025,7 +1031,7 @@
         <v>30</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>31</v>
@@ -1068,13 +1074,13 @@
         <v>24</v>
       </c>
       <c r="D11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="F11" s="16" t="s">
         <v>44</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>45</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>13</v>
@@ -1091,13 +1097,13 @@
         <v>24</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>46</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>47</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>13</v>
@@ -1114,13 +1120,17 @@
         <v>24</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
+        <v>50</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1133,13 +1143,17 @@
         <v>24</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
+      <c r="F14" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>

</xml_diff>